<commit_message>
Update logic to append the url
</commit_message>
<xml_diff>
--- a/Reports/stack_overflow_results.xlsx
+++ b/Reports/stack_overflow_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,41 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>https://stackoverflow.co/teams/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.co/talent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.co/advertising/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.co/labs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.co/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>https://stackoverflow.com/users/20448384/balkrishna-oli</t>
         </is>
       </c>

</xml_diff>

<commit_message>
URL exported from results div with the help of beautifulsoup
</commit_message>
<xml_diff>
--- a/Reports/stack_overflow_results.xlsx
+++ b/Reports/stack_overflow_results.xlsx
@@ -443,70 +443,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/search?q=python+automation#</t>
+          <t>https://stackoverflow.com/questions/50815522/selenium-python-automation?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/</t>
+          <t>https://stackoverflow.com/questions/tagged/python</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/search?q=python+automation#</t>
+          <t>https://stackoverflow.com/questions/tagged/selenium</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/</t>
+          <t>https://stackoverflow.com/questions/tagged/web-crawler</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://stackoverflow.co/teams/</t>
+          <t>https://stackoverflow.com/users/9834021/vidhya</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://stackoverflow.co/talent/</t>
+          <t>https://stackoverflow.com/users/9834021/vidhya</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://stackoverflow.co/advertising/</t>
+          <t>https://stackoverflow.com/questions/43637687/python-automation?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://stackoverflow.co/labs/</t>
+          <t>https://stackoverflow.com/questions/tagged/python</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://stackoverflow.co/</t>
+          <t>https://stackoverflow.com/questions/tagged/selenium</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/users/20448384/balkrishna-oli</t>
+          <t>https://stackoverflow.com/questions/tagged/automation</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added the logic to only grab the results url
There was issue with earlier logic since it is scrabbing other urls like tags url, user profil url and etc
</commit_message>
<xml_diff>
--- a/Reports/stack_overflow_results.xlsx
+++ b/Reports/stack_overflow_results.xlsx
@@ -450,63 +450,63 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/python</t>
+          <t>https://stackoverflow.com/questions/43637687/python-automation?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/selenium</t>
+          <t>https://stackoverflow.com/questions/63717551/how-to-use-python-automation-in-flutter-app?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/web-crawler</t>
+          <t>https://stackoverflow.com/questions/51451268/error-while-exeutiing-selenium-python-automation-script?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/users/9834021/vidhya</t>
+          <t>https://stackoverflow.com/questions/60994919/deploying-a-python-automation-script-in-the-cloud?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/users/9834021/vidhya</t>
+          <t>https://stackoverflow.com/questions/40208051/selenium-using-python-geckodriver-executable-needs-to-be-in-path?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/43637687/python-automation?r=SearchResults</t>
+          <t>https://stackoverflow.com/questions/37048354/python-automation-for-android?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/python</t>
+          <t>https://stackoverflow.com/questions/71252278/calculating-server-throughput-for-selenium-python-automation-test?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/selenium</t>
+          <t>https://stackoverflow.com/questions/77147730/python-automation-using-selenium?r=SearchResults</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://stackoverflow.com/questions/tagged/automation</t>
+          <t>https://stackoverflow.com/questions/40914325/python-automation-using-subprocess?r=SearchResults</t>
         </is>
       </c>
     </row>

</xml_diff>